<commit_message>
change classification of VECA as other (endothelial as description, taxonomy as smooth muscle
</commit_message>
<xml_diff>
--- a/data/single-cell/zeisel_2018/expanded.mmc3.xlsx
+++ b/data/single-cell/zeisel_2018/expanded.mmc3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/data/single-cell/zeisel_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{F399EDFA-C1D6-2E4E-9C88-52D6AD18357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B978D254-2624-CB4F-B301-E1038D7C0B6B}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{F399EDFA-C1D6-2E4E-9C88-52D6AD18357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6838845-5D81-EA41-882E-58F932452644}"/>
   <bookViews>
     <workbookView xWindow="32380" yWindow="-9540" windowWidth="27780" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2924,10 +2924,10 @@
   <dimension ref="A1:J266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D242" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D237" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C264" sqref="C264"/>
+      <selection pane="bottomRight" activeCell="F255" sqref="F255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10515,7 +10515,7 @@
         <v>34</v>
       </c>
       <c r="F255" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I255" s="13" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
change OBDOP cluster name to OBDOP1 to match loom file
</commit_message>
<xml_diff>
--- a/data/single-cell/zeisel_2018/expanded.mmc3.xlsx
+++ b/data/single-cell/zeisel_2018/expanded.mmc3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/data/single-cell/zeisel_2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{F399EDFA-C1D6-2E4E-9C88-52D6AD18357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6838845-5D81-EA41-882E-58F932452644}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{F399EDFA-C1D6-2E4E-9C88-52D6AD18357C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F4407D5-73C1-CE4D-A281-B1C99D021795}"/>
   <bookViews>
-    <workbookView xWindow="32380" yWindow="-9540" windowWidth="27780" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33180" yWindow="-2060" windowWidth="27780" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="7571_0_celltypes_summary_leafor" sheetId="1" r:id="rId1"/>
@@ -2004,9 +2004,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>OBDOP</t>
-  </si>
-  <si>
     <t>Trinarization detects GABA</t>
   </si>
   <si>
@@ -2095,6 +2092,9 @@
   </si>
   <si>
     <t>endothelia</t>
+  </si>
+  <si>
+    <t>OBDOP1</t>
   </si>
 </sst>
 </file>
@@ -2924,10 +2924,10 @@
   <dimension ref="A1:J266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D237" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F255" sqref="F255"/>
+      <selection pane="bottomRight" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2961,7 +2961,7 @@
         <v>596</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>2</v>
@@ -2993,10 +2993,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>626</v>
@@ -3025,7 +3025,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>82</v>
@@ -3054,7 +3054,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>82</v>
@@ -3083,7 +3083,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>82</v>
@@ -3115,7 +3115,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>82</v>
@@ -3144,10 +3144,10 @@
         <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>185</v>
@@ -3173,7 +3173,7 @@
         <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>82</v>
@@ -3205,10 +3205,10 @@
         <v>19</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="13" t="s">
@@ -3235,10 +3235,10 @@
         <v>19</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="13" t="s">
@@ -3265,10 +3265,10 @@
         <v>19</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H11" s="14" t="s">
         <v>627</v>
@@ -3297,10 +3297,10 @@
         <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>625</v>
@@ -3329,10 +3329,10 @@
         <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>630</v>
@@ -3361,10 +3361,10 @@
         <v>19</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="13" t="s">
@@ -3391,10 +3391,10 @@
         <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="13" t="s">
@@ -3421,10 +3421,10 @@
         <v>19</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="13" t="s">
@@ -3451,10 +3451,10 @@
         <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H17" s="14" t="s">
         <v>625</v>
@@ -3483,10 +3483,10 @@
         <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>625</v>
@@ -3515,10 +3515,10 @@
         <v>19</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="13" t="s">
@@ -3545,7 +3545,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>82</v>
@@ -3575,10 +3575,10 @@
         <v>19</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="13" t="s">
@@ -3605,7 +3605,7 @@
         <v>19</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>613</v>
@@ -3635,10 +3635,10 @@
         <v>19</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>629</v>
@@ -3667,7 +3667,7 @@
         <v>19</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>613</v>
@@ -3699,7 +3699,7 @@
         <v>19</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>613</v>
@@ -3731,7 +3731,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>82</v>
@@ -3761,7 +3761,7 @@
         <v>19</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>82</v>
@@ -3791,7 +3791,7 @@
         <v>19</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>94</v>
@@ -3821,7 +3821,7 @@
         <v>19</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>94</v>
@@ -3850,7 +3850,7 @@
         <v>19</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>94</v>
@@ -3879,7 +3879,7 @@
         <v>19</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>94</v>
@@ -3909,7 +3909,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>94</v>
@@ -3938,7 +3938,7 @@
         <v>19</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>94</v>
@@ -3967,7 +3967,7 @@
         <v>78</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>86</v>
@@ -3999,7 +3999,7 @@
         <v>19</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>82</v>
@@ -4031,7 +4031,7 @@
         <v>19</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>86</v>
@@ -4061,7 +4061,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>94</v>
@@ -4091,7 +4091,7 @@
         <v>19</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>94</v>
@@ -4120,7 +4120,7 @@
         <v>19</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>94</v>
@@ -4141,7 +4141,7 @@
         <v>515</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>18</v>
@@ -4150,7 +4150,7 @@
         <v>19</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G40" s="7" t="s">
         <v>94</v>
@@ -4182,7 +4182,7 @@
         <v>19</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>94</v>
@@ -4211,7 +4211,7 @@
         <v>19</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>94</v>
@@ -4241,7 +4241,7 @@
         <v>19</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>94</v>
@@ -4271,7 +4271,7 @@
         <v>19</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>94</v>
@@ -4301,7 +4301,7 @@
         <v>19</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>94</v>
@@ -4319,7 +4319,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>654</v>
+        <v>684</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>277</v>
@@ -4331,7 +4331,7 @@
         <v>19</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G46" s="25" t="s">
         <v>210</v>
@@ -4349,7 +4349,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>278</v>
@@ -4361,7 +4361,7 @@
         <v>19</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>94</v>
@@ -4391,7 +4391,7 @@
         <v>78</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>94</v>
@@ -4423,7 +4423,7 @@
         <v>78</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>94</v>
@@ -4453,7 +4453,7 @@
         <v>19</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>94</v>
@@ -4485,7 +4485,7 @@
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>614</v>
@@ -4515,7 +4515,7 @@
         <v>19</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G52" s="7" t="s">
         <v>94</v>
@@ -4545,7 +4545,7 @@
         <v>19</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G53" s="7" t="s">
         <v>614</v>
@@ -4577,7 +4577,7 @@
         <v>19</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G54" s="7" t="s">
         <v>614</v>
@@ -4607,7 +4607,7 @@
         <v>19</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>614</v>
@@ -4637,7 +4637,7 @@
         <v>19</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>94</v>
@@ -4669,7 +4669,7 @@
         <v>19</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G57" s="7" t="s">
         <v>94</v>
@@ -4699,7 +4699,7 @@
         <v>19</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G58" s="7" t="s">
         <v>615</v>
@@ -4731,7 +4731,7 @@
         <v>19</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>615</v>
@@ -4763,7 +4763,7 @@
         <v>19</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G60" s="7" t="s">
         <v>94</v>
@@ -4793,7 +4793,7 @@
         <v>19</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>615</v>
@@ -4825,7 +4825,7 @@
         <v>19</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>615</v>
@@ -4857,7 +4857,7 @@
         <v>19</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G63" s="7" t="s">
         <v>94</v>
@@ -4887,7 +4887,7 @@
         <v>19</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G64" s="7" t="s">
         <v>614</v>
@@ -4917,7 +4917,7 @@
         <v>19</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G65" s="7" t="s">
         <v>94</v>
@@ -4947,7 +4947,7 @@
         <v>19</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>94</v>
@@ -4977,7 +4977,7 @@
         <v>19</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>94</v>
@@ -5009,7 +5009,7 @@
         <v>19</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G68" s="7" t="s">
         <v>616</v>
@@ -5041,7 +5041,7 @@
         <v>78</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G69" s="7" t="s">
         <v>616</v>
@@ -5073,7 +5073,7 @@
         <v>41</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>617</v>
@@ -5105,10 +5105,10 @@
         <v>41</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H71" s="7" t="s">
         <v>642</v>
@@ -5137,10 +5137,10 @@
         <v>41</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H72" s="7" t="s">
         <v>632</v>
@@ -5169,10 +5169,10 @@
         <v>41</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H73" s="15" t="s">
         <v>643</v>
@@ -5201,7 +5201,7 @@
         <v>78</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G74" s="7" t="s">
         <v>86</v>
@@ -5231,7 +5231,7 @@
         <v>78</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>618</v>
@@ -5263,10 +5263,10 @@
         <v>46</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H76" s="7" t="s">
         <v>632</v>
@@ -5295,7 +5295,7 @@
         <v>46</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>619</v>
@@ -5325,7 +5325,7 @@
         <v>46</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G78" s="7" t="s">
         <v>619</v>
@@ -5355,10 +5355,10 @@
         <v>41</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H79" s="7" t="s">
         <v>625</v>
@@ -5387,10 +5387,10 @@
         <v>41</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H80" s="7" t="s">
         <v>625</v>
@@ -5419,7 +5419,7 @@
         <v>41</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>634</v>
@@ -5451,10 +5451,10 @@
         <v>41</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H82" s="7"/>
       <c r="I82" s="13" t="s">
@@ -5481,10 +5481,10 @@
         <v>41</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H83" s="7" t="s">
         <v>632</v>
@@ -5513,7 +5513,7 @@
         <v>19</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G84" s="7" t="s">
         <v>94</v>
@@ -5543,7 +5543,7 @@
         <v>19</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G85" s="7" t="s">
         <v>94</v>
@@ -5573,7 +5573,7 @@
         <v>78</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>614</v>
@@ -5603,7 +5603,7 @@
         <v>78</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G87" s="7" t="s">
         <v>94</v>
@@ -5633,13 +5633,13 @@
         <v>78</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G88" s="7" t="s">
         <v>618</v>
       </c>
       <c r="H88" s="25" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I88" s="13" t="s">
         <v>315</v>
@@ -5665,7 +5665,7 @@
         <v>78</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G89" s="7" t="s">
         <v>86</v>
@@ -5697,7 +5697,7 @@
         <v>78</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G90" s="7" t="s">
         <v>618</v>
@@ -5729,7 +5729,7 @@
         <v>46</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>94</v>
@@ -5759,7 +5759,7 @@
         <v>78</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>94</v>
@@ -5789,7 +5789,7 @@
         <v>78</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>94</v>
@@ -5819,7 +5819,7 @@
         <v>78</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G94" s="7" t="s">
         <v>94</v>
@@ -5849,7 +5849,7 @@
         <v>78</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G95" s="7" t="s">
         <v>86</v>
@@ -5879,7 +5879,7 @@
         <v>78</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G96" s="7" t="s">
         <v>618</v>
@@ -5909,7 +5909,7 @@
         <v>78</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G97" s="7" t="s">
         <v>86</v>
@@ -5939,7 +5939,7 @@
         <v>67</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G98" s="7" t="s">
         <v>94</v>
@@ -5969,7 +5969,7 @@
         <v>67</v>
       </c>
       <c r="F99" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G99" s="25" t="s">
         <v>620</v>
@@ -6001,7 +6001,7 @@
         <v>67</v>
       </c>
       <c r="F100" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G100" s="25" t="s">
         <v>621</v>
@@ -6033,7 +6033,7 @@
         <v>67</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G101" s="7" t="s">
         <v>94</v>
@@ -6063,7 +6063,7 @@
         <v>67</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G102" s="7" t="s">
         <v>94</v>
@@ -6093,7 +6093,7 @@
         <v>67</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G103" s="7" t="s">
         <v>94</v>
@@ -6123,7 +6123,7 @@
         <v>67</v>
       </c>
       <c r="F104" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G104" s="25" t="s">
         <v>621</v>
@@ -6153,7 +6153,7 @@
         <v>67</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G105" s="7" t="s">
         <v>94</v>
@@ -6183,7 +6183,7 @@
         <v>67</v>
       </c>
       <c r="F106" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G106" s="25" t="s">
         <v>621</v>
@@ -6213,7 +6213,7 @@
         <v>41</v>
       </c>
       <c r="F107" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G107" s="25" t="s">
         <v>621</v>
@@ -6245,7 +6245,7 @@
         <v>67</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>621</v>
@@ -6277,7 +6277,7 @@
         <v>67</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G109" s="7" t="s">
         <v>86</v>
@@ -6307,7 +6307,7 @@
         <v>67</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G110" s="7" t="s">
         <v>86</v>
@@ -6337,7 +6337,7 @@
         <v>67</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G111" s="7" t="s">
         <v>86</v>
@@ -6367,7 +6367,7 @@
         <v>67</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G112" s="7" t="s">
         <v>618</v>
@@ -6397,7 +6397,7 @@
         <v>67</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G113" s="7" t="s">
         <v>86</v>
@@ -6427,7 +6427,7 @@
         <v>67</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G114" s="7" t="s">
         <v>86</v>
@@ -6457,7 +6457,7 @@
         <v>67</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G115" s="7" t="s">
         <v>86</v>
@@ -6487,7 +6487,7 @@
         <v>67</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G116" s="7" t="s">
         <v>86</v>
@@ -6519,7 +6519,7 @@
         <v>67</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G117" s="7" t="s">
         <v>86</v>
@@ -6549,7 +6549,7 @@
         <v>67</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G118" s="7" t="s">
         <v>86</v>
@@ -6579,7 +6579,7 @@
         <v>41</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G119" s="7" t="s">
         <v>86</v>
@@ -6609,7 +6609,7 @@
         <v>41</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G120" s="7" t="s">
         <v>618</v>
@@ -6641,7 +6641,7 @@
         <v>41</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>618</v>
@@ -6671,7 +6671,7 @@
         <v>46</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>86</v>
@@ -6701,7 +6701,7 @@
         <v>46</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>86</v>
@@ -6731,7 +6731,7 @@
         <v>46</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>86</v>
@@ -6761,7 +6761,7 @@
         <v>46</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G125" s="4" t="s">
         <v>86</v>
@@ -6793,7 +6793,7 @@
         <v>46</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G126" s="4" t="s">
         <v>86</v>
@@ -6822,7 +6822,7 @@
         <v>46</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G127" s="4" t="s">
         <v>618</v>
@@ -6851,7 +6851,7 @@
         <v>46</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>618</v>
@@ -6883,7 +6883,7 @@
         <v>46</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G129" s="4" t="s">
         <v>618</v>
@@ -6912,7 +6912,7 @@
         <v>46</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G130" s="4" t="s">
         <v>86</v>
@@ -6942,7 +6942,7 @@
         <v>46</v>
       </c>
       <c r="F131" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G131" s="25" t="s">
         <v>226</v>
@@ -6971,7 +6971,7 @@
         <v>46</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G132" s="4" t="s">
         <v>86</v>
@@ -7000,7 +7000,7 @@
         <v>46</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G133" s="4" t="s">
         <v>86</v>
@@ -7030,7 +7030,7 @@
         <v>46</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G134" s="4" t="s">
         <v>618</v>
@@ -7059,10 +7059,10 @@
         <v>19</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H135" s="7"/>
       <c r="I135" s="13" t="s">
@@ -7089,10 +7089,10 @@
         <v>78</v>
       </c>
       <c r="F136" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G136" s="25" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H136" s="4" t="s">
         <v>645</v>
@@ -7121,10 +7121,10 @@
         <v>41</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G137" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H137" s="7"/>
       <c r="I137" s="13" t="s">
@@ -7151,10 +7151,10 @@
         <v>78</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G138" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I138" s="13" t="s">
         <v>313</v>
@@ -7180,10 +7180,10 @@
         <v>78</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G139" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H139" s="7" t="s">
         <v>638</v>
@@ -7212,7 +7212,7 @@
         <v>78</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G140" s="4" t="s">
         <v>86</v>
@@ -7241,10 +7241,10 @@
         <v>78</v>
       </c>
       <c r="F141" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I141" s="13" t="s">
         <v>313</v>
@@ -7270,7 +7270,7 @@
         <v>46</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G142" s="4" t="s">
         <v>94</v>
@@ -7300,7 +7300,7 @@
         <v>46</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G143" s="4" t="s">
         <v>614</v>
@@ -7330,7 +7330,7 @@
         <v>46</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>614</v>
@@ -7359,7 +7359,7 @@
         <v>46</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G145" s="4" t="s">
         <v>94</v>
@@ -7391,7 +7391,7 @@
         <v>46</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G146" s="4" t="s">
         <v>94</v>
@@ -7421,7 +7421,7 @@
         <v>46</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G147" s="4" t="s">
         <v>94</v>
@@ -7453,7 +7453,7 @@
         <v>46</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G148" s="4" t="s">
         <v>94</v>
@@ -7483,7 +7483,7 @@
         <v>46</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G149" s="4" t="s">
         <v>614</v>
@@ -7513,7 +7513,7 @@
         <v>46</v>
       </c>
       <c r="F150" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G150" s="4" t="s">
         <v>94</v>
@@ -7543,7 +7543,7 @@
         <v>41</v>
       </c>
       <c r="F151" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G151" s="25" t="s">
         <v>621</v>
@@ -7573,7 +7573,7 @@
         <v>46</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G152" s="4" t="s">
         <v>94</v>
@@ -7603,7 +7603,7 @@
         <v>78</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G153" s="4" t="s">
         <v>94</v>
@@ -7633,7 +7633,7 @@
         <v>19</v>
       </c>
       <c r="F154" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G154" s="4" t="s">
         <v>94</v>
@@ -7663,7 +7663,7 @@
         <v>46</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G155" s="4" t="s">
         <v>94</v>
@@ -7693,7 +7693,7 @@
         <v>46</v>
       </c>
       <c r="F156" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G156" s="4" t="s">
         <v>94</v>
@@ -7725,7 +7725,7 @@
         <v>41</v>
       </c>
       <c r="F157" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G157" s="4" t="s">
         <v>614</v>
@@ -7754,7 +7754,7 @@
         <v>41</v>
       </c>
       <c r="F158" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G158" s="26" t="s">
         <v>621</v>
@@ -7786,7 +7786,7 @@
         <v>41</v>
       </c>
       <c r="F159" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G159" s="25" t="s">
         <v>621</v>
@@ -7818,7 +7818,7 @@
         <v>41</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G160" s="4" t="s">
         <v>621</v>
@@ -7850,7 +7850,7 @@
         <v>41</v>
       </c>
       <c r="F161" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G161" s="25" t="s">
         <v>622</v>
@@ -7882,10 +7882,10 @@
         <v>41</v>
       </c>
       <c r="F162" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G162" s="25" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I162" s="13" t="s">
         <v>129</v>
@@ -7911,10 +7911,10 @@
         <v>41</v>
       </c>
       <c r="F163" s="24" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G163" s="25" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H163" s="25" t="s">
         <v>650</v>
@@ -7943,10 +7943,10 @@
         <v>41</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G164" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H164" s="7"/>
       <c r="I164" s="13" t="s">
@@ -7973,10 +7973,10 @@
         <v>41</v>
       </c>
       <c r="F165" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G165" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I165" s="13" t="s">
         <v>129</v>
@@ -8002,10 +8002,10 @@
         <v>41</v>
       </c>
       <c r="F166" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G166" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H166" s="7" t="s">
         <v>636</v>
@@ -8034,10 +8034,10 @@
         <v>41</v>
       </c>
       <c r="F167" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G167" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I167" s="13" t="s">
         <v>129</v>
@@ -8063,10 +8063,10 @@
         <v>41</v>
       </c>
       <c r="F168" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G168" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H168" s="7"/>
       <c r="I168" s="13" t="s">
@@ -8093,10 +8093,10 @@
         <v>41</v>
       </c>
       <c r="F169" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G169" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H169" s="7" t="s">
         <v>646</v>
@@ -8125,7 +8125,7 @@
         <v>41</v>
       </c>
       <c r="F170" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G170" s="25" t="s">
         <v>621</v>
@@ -8157,7 +8157,7 @@
         <v>41</v>
       </c>
       <c r="F171" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G171" s="25" t="s">
         <v>621</v>
@@ -8187,7 +8187,7 @@
         <v>67</v>
       </c>
       <c r="F172" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G172" s="25" t="s">
         <v>621</v>
@@ -8216,7 +8216,7 @@
         <v>41</v>
       </c>
       <c r="F173" s="24" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G173" s="25" t="s">
         <v>621</v>
@@ -8245,7 +8245,7 @@
         <v>46</v>
       </c>
       <c r="F174" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G174" s="4" t="s">
         <v>614</v>
@@ -8275,7 +8275,7 @@
         <v>41</v>
       </c>
       <c r="F175" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G175" s="4" t="s">
         <v>614</v>
@@ -8304,7 +8304,7 @@
         <v>41</v>
       </c>
       <c r="F176" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G176" s="22" t="s">
         <v>94</v>
@@ -8336,7 +8336,7 @@
         <v>41</v>
       </c>
       <c r="F177" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G177" s="4" t="s">
         <v>82</v>
@@ -8365,7 +8365,7 @@
         <v>41</v>
       </c>
       <c r="F178" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G178" s="4" t="s">
         <v>82</v>
@@ -8395,10 +8395,10 @@
         <v>41</v>
       </c>
       <c r="F179" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G179" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H179" s="7"/>
       <c r="I179" s="13" t="s">
@@ -8425,10 +8425,10 @@
         <v>19</v>
       </c>
       <c r="F180" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G180" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H180" s="7"/>
       <c r="I180" s="13" t="s">
@@ -8455,10 +8455,10 @@
         <v>19</v>
       </c>
       <c r="F181" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G181" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H181" s="7"/>
       <c r="I181" s="13" t="s">
@@ -8485,10 +8485,10 @@
         <v>19</v>
       </c>
       <c r="F182" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G182" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H182" s="7" t="s">
         <v>639</v>
@@ -8517,7 +8517,7 @@
         <v>23</v>
       </c>
       <c r="F183" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G183" s="4" t="s">
         <v>623</v>
@@ -8546,10 +8546,10 @@
         <v>23</v>
       </c>
       <c r="F184" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G184" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H184" s="7"/>
       <c r="I184" s="13" t="s">
@@ -8576,10 +8576,10 @@
         <v>23</v>
       </c>
       <c r="F185" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G185" s="4" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H185" s="7"/>
       <c r="I185" s="13" t="s">
@@ -8606,7 +8606,7 @@
         <v>23</v>
       </c>
       <c r="F186" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G186" s="4" t="s">
         <v>123</v>
@@ -8635,7 +8635,7 @@
         <v>23</v>
       </c>
       <c r="F187" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G187" s="4" t="s">
         <v>123</v>
@@ -8664,7 +8664,7 @@
         <v>23</v>
       </c>
       <c r="F188" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G188" s="22" t="s">
         <v>123</v>
@@ -8694,7 +8694,7 @@
         <v>23</v>
       </c>
       <c r="F189" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G189" s="22" t="s">
         <v>226</v>
@@ -8726,7 +8726,7 @@
         <v>23</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G190" s="22" t="s">
         <v>226</v>
@@ -8756,7 +8756,7 @@
         <v>23</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G191" s="4" t="s">
         <v>123</v>
@@ -8785,7 +8785,7 @@
         <v>23</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G192" s="4" t="s">
         <v>155</v>
@@ -8815,7 +8815,7 @@
         <v>23</v>
       </c>
       <c r="F193" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G193" s="4" t="s">
         <v>155</v>
@@ -8844,7 +8844,7 @@
         <v>23</v>
       </c>
       <c r="F194" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G194" s="4" t="s">
         <v>155</v>
@@ -8873,7 +8873,7 @@
         <v>23</v>
       </c>
       <c r="F195" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G195" s="4" t="s">
         <v>155</v>
@@ -8902,7 +8902,7 @@
         <v>23</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G196" s="4" t="s">
         <v>155</v>
@@ -8931,7 +8931,7 @@
         <v>23</v>
       </c>
       <c r="F197" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G197" s="4" t="s">
         <v>624</v>
@@ -8960,7 +8960,7 @@
         <v>23</v>
       </c>
       <c r="F198" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G198" s="4" t="s">
         <v>624</v>
@@ -8989,7 +8989,7 @@
         <v>23</v>
       </c>
       <c r="F199" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G199" s="4" t="s">
         <v>86</v>
@@ -9019,7 +9019,7 @@
         <v>23</v>
       </c>
       <c r="F200" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G200" s="4" t="s">
         <v>86</v>
@@ -9048,7 +9048,7 @@
         <v>23</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G201" s="4" t="s">
         <v>86</v>
@@ -9077,7 +9077,7 @@
         <v>23</v>
       </c>
       <c r="F202" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G202" s="4" t="s">
         <v>86</v>
@@ -9107,7 +9107,7 @@
         <v>23</v>
       </c>
       <c r="F203" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G203" s="4" t="s">
         <v>618</v>
@@ -9137,7 +9137,7 @@
         <v>23</v>
       </c>
       <c r="F204" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G204" s="4" t="s">
         <v>86</v>
@@ -9167,7 +9167,7 @@
         <v>23</v>
       </c>
       <c r="F205" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G205" s="4" t="s">
         <v>86</v>
@@ -9197,10 +9197,10 @@
         <v>23</v>
       </c>
       <c r="F206" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G206" s="4" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H206" s="7" t="s">
         <v>639</v>
@@ -9229,10 +9229,10 @@
         <v>23</v>
       </c>
       <c r="F207" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G207" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H207" s="7"/>
       <c r="I207" s="13" t="s">
@@ -9259,10 +9259,10 @@
         <v>23</v>
       </c>
       <c r="F208" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H208" s="7" t="s">
         <v>625</v>
@@ -9291,10 +9291,10 @@
         <v>23</v>
       </c>
       <c r="F209" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G209" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>625</v>
@@ -9323,10 +9323,10 @@
         <v>23</v>
       </c>
       <c r="F210" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G210" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="H210" s="7"/>
       <c r="I210" s="13" t="s">
@@ -9353,7 +9353,7 @@
         <v>23</v>
       </c>
       <c r="F211" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G211" s="4" t="s">
         <v>86</v>
@@ -9382,7 +9382,7 @@
         <v>23</v>
       </c>
       <c r="F212" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G212" s="4" t="s">
         <v>86</v>
@@ -9411,7 +9411,7 @@
         <v>23</v>
       </c>
       <c r="F213" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G213" s="4" t="s">
         <v>86</v>
@@ -9441,7 +9441,7 @@
         <v>23</v>
       </c>
       <c r="F214" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G214" s="4" t="s">
         <v>86</v>
@@ -9471,7 +9471,7 @@
         <v>23</v>
       </c>
       <c r="F215" s="5" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G215" s="4" t="s">
         <v>86</v>
@@ -9500,7 +9500,7 @@
         <v>5</v>
       </c>
       <c r="F216" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H216" s="7"/>
       <c r="I216" s="13" t="s">
@@ -9527,7 +9527,7 @@
         <v>5</v>
       </c>
       <c r="F217" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I217" s="13" t="s">
         <v>6</v>
@@ -9553,7 +9553,7 @@
         <v>5</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I218" s="13" t="s">
         <v>6</v>
@@ -9579,7 +9579,7 @@
         <v>5</v>
       </c>
       <c r="F219" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I219" s="13" t="s">
         <v>6</v>
@@ -9605,7 +9605,7 @@
         <v>5</v>
       </c>
       <c r="F220" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I220" s="13" t="s">
         <v>6</v>
@@ -9631,7 +9631,7 @@
         <v>5</v>
       </c>
       <c r="F221" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I221" s="13" t="s">
         <v>6</v>
@@ -9657,7 +9657,7 @@
         <v>5</v>
       </c>
       <c r="F222" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I222" s="13" t="s">
         <v>6</v>
@@ -9683,7 +9683,7 @@
         <v>5</v>
       </c>
       <c r="F223" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I223" s="13" t="s">
         <v>6</v>
@@ -9709,7 +9709,7 @@
         <v>5</v>
       </c>
       <c r="F224" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I224" s="13" t="s">
         <v>6</v>
@@ -9735,7 +9735,7 @@
         <v>5</v>
       </c>
       <c r="F225" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I225" s="13" t="s">
         <v>75</v>
@@ -9761,7 +9761,7 @@
         <v>5</v>
       </c>
       <c r="F226" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I226" s="5" t="s">
         <v>71</v>
@@ -9787,7 +9787,7 @@
         <v>5</v>
       </c>
       <c r="F227" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I227" s="13" t="s">
         <v>64</v>
@@ -9813,7 +9813,7 @@
         <v>5</v>
       </c>
       <c r="F228" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I228" s="13" t="s">
         <v>64</v>
@@ -9839,7 +9839,7 @@
         <v>46</v>
       </c>
       <c r="F229" s="6" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I229" s="13" t="s">
         <v>64</v>
@@ -9865,7 +9865,7 @@
         <v>19</v>
       </c>
       <c r="F230" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I230" s="13" t="s">
         <v>60</v>
@@ -9891,7 +9891,7 @@
         <v>19</v>
       </c>
       <c r="F231" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I231" s="13" t="s">
         <v>56</v>
@@ -9917,7 +9917,7 @@
         <v>19</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I232" s="13" t="s">
         <v>17</v>
@@ -9943,7 +9943,7 @@
         <v>19</v>
       </c>
       <c r="F233" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I233" s="13" t="s">
         <v>17</v>
@@ -9969,7 +9969,7 @@
         <v>19</v>
       </c>
       <c r="F234" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I234" s="13" t="s">
         <v>17</v>
@@ -9995,7 +9995,7 @@
         <v>51</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I235" s="13" t="s">
         <v>17</v>
@@ -10021,7 +10021,7 @@
         <v>51</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I236" s="13" t="s">
         <v>17</v>
@@ -10047,7 +10047,7 @@
         <v>46</v>
       </c>
       <c r="F237" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I237" s="13" t="s">
         <v>17</v>
@@ -10073,7 +10073,7 @@
         <v>41</v>
       </c>
       <c r="F238" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I238" s="13" t="s">
         <v>17</v>
@@ -10099,7 +10099,7 @@
         <v>23</v>
       </c>
       <c r="F239" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I239" s="13" t="s">
         <v>20</v>
@@ -10125,7 +10125,7 @@
         <v>5</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I240" s="13" t="s">
         <v>16</v>
@@ -10151,7 +10151,7 @@
         <v>23</v>
       </c>
       <c r="F241" s="24" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I241" s="13" t="s">
         <v>27</v>
@@ -10177,7 +10177,7 @@
         <v>23</v>
       </c>
       <c r="F242" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I242" s="13" t="s">
         <v>24</v>
@@ -10203,7 +10203,7 @@
         <v>23</v>
       </c>
       <c r="F243" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I243" s="13" t="s">
         <v>24</v>
@@ -10229,7 +10229,7 @@
         <v>23</v>
       </c>
       <c r="F244" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I244" s="13" t="s">
         <v>33</v>
@@ -10255,7 +10255,7 @@
         <v>23</v>
       </c>
       <c r="F245" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I245" s="13" t="s">
         <v>33</v>
@@ -10281,7 +10281,7 @@
         <v>23</v>
       </c>
       <c r="F246" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I246" s="13" t="s">
         <v>33</v>
@@ -10307,7 +10307,7 @@
         <v>23</v>
       </c>
       <c r="F247" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I247" s="13" t="s">
         <v>33</v>
@@ -10333,7 +10333,7 @@
         <v>23</v>
       </c>
       <c r="F248" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I248" s="13" t="s">
         <v>33</v>
@@ -10359,7 +10359,7 @@
         <v>23</v>
       </c>
       <c r="F249" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I249" s="13" t="s">
         <v>33</v>
@@ -10385,7 +10385,7 @@
         <v>23</v>
       </c>
       <c r="F250" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I250" s="13" t="s">
         <v>33</v>
@@ -10411,7 +10411,7 @@
         <v>23</v>
       </c>
       <c r="F251" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I251" s="13" t="s">
         <v>33</v>
@@ -10437,7 +10437,7 @@
         <v>23</v>
       </c>
       <c r="F252" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I252" s="13" t="s">
         <v>29</v>
@@ -10463,7 +10463,7 @@
         <v>23</v>
       </c>
       <c r="F253" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I253" s="13" t="s">
         <v>29</v>
@@ -10489,7 +10489,7 @@
         <v>23</v>
       </c>
       <c r="F254" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I254" s="13" t="s">
         <v>29</v>
@@ -10515,7 +10515,7 @@
         <v>34</v>
       </c>
       <c r="F255" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I255" s="13" t="s">
         <v>35</v>
@@ -10541,7 +10541,7 @@
         <v>34</v>
       </c>
       <c r="F256" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I256" s="13" t="s">
         <v>35</v>
@@ -10567,7 +10567,7 @@
         <v>34</v>
       </c>
       <c r="F257" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I257" s="13" t="s">
         <v>35</v>
@@ -10593,7 +10593,7 @@
         <v>34</v>
       </c>
       <c r="F258" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I258" s="13" t="s">
         <v>36</v>
@@ -10619,7 +10619,7 @@
         <v>34</v>
       </c>
       <c r="F259" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I259" s="13" t="s">
         <v>36</v>
@@ -10645,7 +10645,7 @@
         <v>34</v>
       </c>
       <c r="F260" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I260" s="13" t="s">
         <v>37</v>
@@ -10671,7 +10671,7 @@
         <v>34</v>
       </c>
       <c r="F261" s="5" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I261" s="13" t="s">
         <v>37</v>
@@ -10697,7 +10697,7 @@
         <v>34</v>
       </c>
       <c r="F262" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I262" s="13" t="s">
         <v>38</v>
@@ -10723,7 +10723,7 @@
         <v>34</v>
       </c>
       <c r="F263" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I263" s="13" t="s">
         <v>38</v>
@@ -10749,7 +10749,7 @@
         <v>34</v>
       </c>
       <c r="F264" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I264" s="13" t="s">
         <v>39</v>
@@ -10775,7 +10775,7 @@
         <v>34</v>
       </c>
       <c r="F265" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I265" s="13" t="s">
         <v>39</v>
@@ -10801,7 +10801,7 @@
         <v>34</v>
       </c>
       <c r="F266" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I266" s="13" t="s">
         <v>39</v>
@@ -10825,8 +10825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>